<commit_message>
[update] codes & results of CC
</commit_message>
<xml_diff>
--- a/Results_ConservativeComparison/ConservativeComparison_BlindIntersection.xlsx
+++ b/Results_ConservativeComparison/ConservativeComparison_BlindIntersection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RE2022\RE2022 Supplementary Materials\Results_ConservativeComparison\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Documents\GitHub\Hierarchical-Safety-Assessment\Results_ConservativeComparison\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,10 +27,7 @@
     <t>Configuration B</t>
   </si>
   <si>
-    <t>Comparison</t>
-  </si>
-  <si>
-    <t>20_100000000_250_20_20_3000</t>
+    <t>Comparison Results</t>
   </si>
   <si>
     <t>0.625_100000000_250_20_20_3000</t>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>20_100000000_250_20_20_24000</t>
+  </si>
+  <si>
+    <t>20_100000000_250_20_20_3000</t>
   </si>
   <si>
     <t>20_100000000_250_20_20_375.0</t>
@@ -219,10 +219,10 @@
     <t>A&lt;B</t>
   </si>
   <si>
-    <t>A&gt;B</t>
+    <t>A=B</t>
   </si>
   <si>
-    <t>A=B</t>
+    <t>A&gt;B</t>
   </si>
   <si>
     <t>Configuration B is safer than Configuration A</t>
@@ -238,7 +238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,14 +256,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -305,19 +297,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -623,18 +606,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1831"/>
+  <dimension ref="A1:H1831"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G3"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="7" max="7" width="9" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,14 +624,14 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -664,14 +644,14 @@
       <c r="D2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -684,14 +664,14 @@
       <c r="D3" t="s">
         <v>64</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -704,9 +684,8 @@
       <c r="D4" t="s">
         <v>64</v>
       </c>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -720,7 +699,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -734,7 +713,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -745,10 +724,10 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -762,7 +741,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -776,7 +755,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -790,7 +769,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -804,7 +783,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -818,7 +797,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -832,7 +811,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -846,7 +825,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -860,7 +839,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1249,7 +1228,7 @@
         <v>45</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
@@ -1319,7 +1298,7 @@
         <v>50</v>
       </c>
       <c r="D48" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
@@ -1333,7 +1312,7 @@
         <v>51</v>
       </c>
       <c r="D49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
@@ -1375,7 +1354,7 @@
         <v>54</v>
       </c>
       <c r="D52" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
@@ -1389,7 +1368,7 @@
         <v>55</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
@@ -1431,7 +1410,7 @@
         <v>58</v>
       </c>
       <c r="D56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
@@ -3111,7 +3090,7 @@
         <v>61</v>
       </c>
       <c r="D176" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.15">
@@ -3909,7 +3888,7 @@
         <v>61</v>
       </c>
       <c r="D233" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.15">
@@ -4973,7 +4952,7 @@
         <v>26</v>
       </c>
       <c r="D309" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.15">
@@ -16705,7 +16684,7 @@
         <v>45</v>
       </c>
       <c r="D1147" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1148" spans="1:4" x14ac:dyDescent="0.15">
@@ -16775,7 +16754,7 @@
         <v>50</v>
       </c>
       <c r="D1152" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1153" spans="1:4" x14ac:dyDescent="0.15">
@@ -16789,7 +16768,7 @@
         <v>51</v>
       </c>
       <c r="D1153" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1154" spans="1:4" x14ac:dyDescent="0.15">
@@ -16831,7 +16810,7 @@
         <v>54</v>
       </c>
       <c r="D1156" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1157" spans="1:4" x14ac:dyDescent="0.15">
@@ -16845,7 +16824,7 @@
         <v>55</v>
       </c>
       <c r="D1157" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1158" spans="1:4" x14ac:dyDescent="0.15">
@@ -16887,7 +16866,7 @@
         <v>58</v>
       </c>
       <c r="D1160" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1161" spans="1:4" x14ac:dyDescent="0.15">
@@ -25077,7 +25056,7 @@
         <v>55</v>
       </c>
       <c r="D1745" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1746" spans="1:4" x14ac:dyDescent="0.15">
@@ -25245,7 +25224,7 @@
         <v>55</v>
       </c>
       <c r="D1757" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1758" spans="1:4" x14ac:dyDescent="0.15">
@@ -25665,7 +25644,7 @@
         <v>55</v>
       </c>
       <c r="D1787" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="1788" spans="1:4" x14ac:dyDescent="0.15">
@@ -25819,7 +25798,7 @@
         <v>58</v>
       </c>
       <c r="D1798" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="1799" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>